<commit_message>
1st set of imgs
</commit_message>
<xml_diff>
--- a/public/excel/Skabelon.xlsx
+++ b/public/excel/Skabelon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolaiblakwalther/PhpstormProjects/SmagenAfOl/public/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\PhpstormProjects\SmagenAfOl\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C24BFF-B35D-3F4B-BA06-63916E1A89BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A45199-94DF-46D6-882B-4821A28BFD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{A986B120-36F4-4CAD-BCDD-1D8F0F805847}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A986B120-36F4-4CAD-BCDD-1D8F0F805847}"/>
   </bookViews>
   <sheets>
     <sheet name="Øl" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="354">
   <si>
     <t>name</t>
   </si>
@@ -327,6 +327,9 @@
     <t>Biére De Garde</t>
   </si>
   <si>
+    <t>Imp. Porter</t>
+  </si>
+  <si>
     <t>Whisky &amp; Rye</t>
   </si>
   <si>
@@ -369,9 +372,6 @@
     <t>Champagne Øl</t>
   </si>
   <si>
-    <t>The Stay Puffed</t>
-  </si>
-  <si>
     <t>Krig, Fred &amp; Kærlighed</t>
   </si>
   <si>
@@ -478,6 +478,627 @@
   </si>
   <si>
     <t>destillery</t>
+  </si>
+  <si>
+    <t>sortSolRom.jpeg</t>
+  </si>
+  <si>
+    <t>orangeRom.jpeg</t>
+  </si>
+  <si>
+    <t>nordicRom.jpeg</t>
+  </si>
+  <si>
+    <t>originalGin.jpeg</t>
+  </si>
+  <si>
+    <t>appleGin.jpeg</t>
+  </si>
+  <si>
+    <t>kokosrom.jpeg</t>
+  </si>
+  <si>
+    <t>klitroseGin.jpeg</t>
+  </si>
+  <si>
+    <t>citrusGin.jpeg</t>
+  </si>
+  <si>
+    <t>pinkGrapeGin.jpeg</t>
+  </si>
+  <si>
+    <t>rhubarbGin.jpeg</t>
+  </si>
+  <si>
+    <t>kimerudAged.jpeg</t>
+  </si>
+  <si>
+    <t>kimerudPink.jpeg</t>
+  </si>
+  <si>
+    <t>kimerudGin.jpeg</t>
+  </si>
+  <si>
+    <t>lonewolfGin.jpeg</t>
+  </si>
+  <si>
+    <t>The Stay Puft</t>
+  </si>
+  <si>
+    <t>Remmarslöv Gårdsbryggeri</t>
+  </si>
+  <si>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t>Sourbon</t>
+  </si>
+  <si>
+    <t>Geuzeboon</t>
+  </si>
+  <si>
+    <t>BA Sour</t>
+  </si>
+  <si>
+    <t>BA Ale</t>
+  </si>
+  <si>
+    <t>Boon Brouwerij</t>
+  </si>
+  <si>
+    <t>Indulgence Funken</t>
+  </si>
+  <si>
+    <t>Indulgence Anno 1521</t>
+  </si>
+  <si>
+    <t>Amber Ale</t>
+  </si>
+  <si>
+    <t>Blonde Ale</t>
+  </si>
+  <si>
+    <t>Imperial Dark</t>
+  </si>
+  <si>
+    <t>Dark Ale</t>
+  </si>
+  <si>
+    <t>Classic</t>
+  </si>
+  <si>
+    <t>Ambrio</t>
+  </si>
+  <si>
+    <t>Martha</t>
+  </si>
+  <si>
+    <t>Brown Eyes</t>
+  </si>
+  <si>
+    <t>Poppels Bryggeri</t>
+  </si>
+  <si>
+    <t>All-Into It Stout</t>
+  </si>
+  <si>
+    <t>BA Stout</t>
+  </si>
+  <si>
+    <t>Guilty Pleasure</t>
+  </si>
+  <si>
+    <t>Red Ale</t>
+  </si>
+  <si>
+    <t>Sexy Blond</t>
+  </si>
+  <si>
+    <t>Barrel Aged Stout</t>
+  </si>
+  <si>
+    <t>Rhum &amp; Bourbon Stout</t>
+  </si>
+  <si>
+    <t>Heavy Hitter</t>
+  </si>
+  <si>
+    <t>Lervig</t>
+  </si>
+  <si>
+    <t>Here We Go Again</t>
+  </si>
+  <si>
+    <t>IPA</t>
+  </si>
+  <si>
+    <t>Superfreunde Gym</t>
+  </si>
+  <si>
+    <t>Tilquin</t>
+  </si>
+  <si>
+    <t>Oude Gueuze</t>
+  </si>
+  <si>
+    <t>Oude Quetsche</t>
+  </si>
+  <si>
+    <t>Baristaen</t>
+  </si>
+  <si>
+    <t>Elskerinden</t>
+  </si>
+  <si>
+    <t>Psykopaten</t>
+  </si>
+  <si>
+    <t>Agenten</t>
+  </si>
+  <si>
+    <t>Fyrbøderen</t>
+  </si>
+  <si>
+    <t>Oud Beersel Brewery</t>
+  </si>
+  <si>
+    <t>Vandervelden 137</t>
+  </si>
+  <si>
+    <t>Brouwerij Verhaeghe</t>
+  </si>
+  <si>
+    <t>Duchesse De Bourgogne</t>
+  </si>
+  <si>
+    <t>Whisky Infused</t>
+  </si>
+  <si>
+    <t>Dry &amp; Bitter</t>
+  </si>
+  <si>
+    <t>Mirror Me</t>
+  </si>
+  <si>
+    <t>Ponder On</t>
+  </si>
+  <si>
+    <t>Dwell In The Fog</t>
+  </si>
+  <si>
+    <t>Future Paradox</t>
+  </si>
+  <si>
+    <t>Session IPA</t>
+  </si>
+  <si>
+    <t>Romanoid</t>
+  </si>
+  <si>
+    <t>Double Dippy Doo</t>
+  </si>
+  <si>
+    <t>Optimal Illusion</t>
+  </si>
+  <si>
+    <t>Amundsen</t>
+  </si>
+  <si>
+    <t>Dessert In A Can Triple Berry Pavlova</t>
+  </si>
+  <si>
+    <t>Barrel Aged Dessert In A Can Tonka &amp; Caramel Swirl Ice-Cream</t>
+  </si>
+  <si>
+    <t>Barrel Aged Dessert In A Can Mamma's Blueberry Pie</t>
+  </si>
+  <si>
+    <t>Barrel Aged Dessert In A Can Chocolate Covered Salted Toffee Popcorn</t>
+  </si>
+  <si>
+    <t>Dessert In A Can Raspberry, Salted Caramel Cheesecake</t>
+  </si>
+  <si>
+    <t>Bairisch Pils</t>
+  </si>
+  <si>
+    <t>Kellerbier</t>
+  </si>
+  <si>
+    <t>Urweisse</t>
+  </si>
+  <si>
+    <t>Beirisch Pilsner</t>
+  </si>
+  <si>
+    <t>Celebrator</t>
+  </si>
+  <si>
+    <t>Doppelbock</t>
+  </si>
+  <si>
+    <t>Schneider Weisse</t>
+  </si>
+  <si>
+    <t>Original Weissbier</t>
+  </si>
+  <si>
+    <t>Weissbier</t>
+  </si>
+  <si>
+    <t>Aventinus Weizen-Doppelbock</t>
+  </si>
+  <si>
+    <t>Aventinus Eisbock</t>
+  </si>
+  <si>
+    <t>Rohozec</t>
+  </si>
+  <si>
+    <t>Dvanáctka</t>
+  </si>
+  <si>
+    <t>Trináctka Tmavá</t>
+  </si>
+  <si>
+    <t>Midtfyns Bryghus</t>
+  </si>
+  <si>
+    <t>Russian Imperial Stout</t>
+  </si>
+  <si>
+    <t>Chili Tripel</t>
+  </si>
+  <si>
+    <t>West Brew</t>
+  </si>
+  <si>
+    <t>Winter Warmer 2021</t>
+  </si>
+  <si>
+    <t>Soul Warmer</t>
+  </si>
+  <si>
+    <t>Brown Bourbon Ale</t>
+  </si>
+  <si>
+    <t>Farmhouse Pale Ale</t>
+  </si>
+  <si>
+    <t>Saison Sea Buckthorn &amp; Elderflaower</t>
+  </si>
+  <si>
+    <t>Saison</t>
+  </si>
+  <si>
+    <t>Barrel Aged Strong Ale</t>
+  </si>
+  <si>
+    <t>Black Night</t>
+  </si>
+  <si>
+    <t>Porter</t>
+  </si>
+  <si>
+    <t>Have Space Suit - Will Travel</t>
+  </si>
+  <si>
+    <t>flygtning.jpeg</t>
+  </si>
+  <si>
+    <t>varmoel.jpeg</t>
+  </si>
+  <si>
+    <t>oats.jpeg</t>
+  </si>
+  <si>
+    <t>rainbows.jpeg</t>
+  </si>
+  <si>
+    <t>spontan.jpeg</t>
+  </si>
+  <si>
+    <t>covfefeStd.jpeg</t>
+  </si>
+  <si>
+    <t>covfefeElg.jpeg</t>
+  </si>
+  <si>
+    <t>covfefeWhisky.jpeg</t>
+  </si>
+  <si>
+    <t>covfefeEg.jpeg</t>
+  </si>
+  <si>
+    <t>grauballeBock.jpeg</t>
+  </si>
+  <si>
+    <t>herslevPaaske.jpeg</t>
+  </si>
+  <si>
+    <t>aeroePaaske.jpeg</t>
+  </si>
+  <si>
+    <t>ayingerPils.jpeg</t>
+  </si>
+  <si>
+    <t>whiteWedding.jpeg</t>
+  </si>
+  <si>
+    <t>goudenEaster.jpeg</t>
+  </si>
+  <si>
+    <t>gorm.jpeg</t>
+  </si>
+  <si>
+    <t>redWedding.jpeg</t>
+  </si>
+  <si>
+    <t>margeret.jpeg</t>
+  </si>
+  <si>
+    <t>1741.jpeg</t>
+  </si>
+  <si>
+    <t>fanoeWAR.jpeg</t>
+  </si>
+  <si>
+    <t>mussolini.jpeg</t>
+  </si>
+  <si>
+    <t>bringBrown.jpeg</t>
+  </si>
+  <si>
+    <t>15imp.jpeg</t>
+  </si>
+  <si>
+    <t>farFromKoln.jpeg</t>
+  </si>
+  <si>
+    <t>bringOak.jpeg</t>
+  </si>
+  <si>
+    <t>bigBang2022.jpeg</t>
+  </si>
+  <si>
+    <t>puft.jpeg</t>
+  </si>
+  <si>
+    <t>krigFred.jpeg</t>
+  </si>
+  <si>
+    <t>600.jpeg</t>
+  </si>
+  <si>
+    <t>olaDubh12.jpeg</t>
+  </si>
+  <si>
+    <t>olaDubh14.jpeg</t>
+  </si>
+  <si>
+    <t>olaDubh16.jpeg</t>
+  </si>
+  <si>
+    <t>olaDubh18.jpeg</t>
+  </si>
+  <si>
+    <t>olaDubh21.jpeg</t>
+  </si>
+  <si>
+    <t>matryoshka.jpeg</t>
+  </si>
+  <si>
+    <t>pepper.jpeg</t>
+  </si>
+  <si>
+    <t>fermento.jpeg</t>
+  </si>
+  <si>
+    <t>catSkill.jpeg</t>
+  </si>
+  <si>
+    <t>grandOpening.jpeg</t>
+  </si>
+  <si>
+    <t>hel.jpeg</t>
+  </si>
+  <si>
+    <t>said.jpeg</t>
+  </si>
+  <si>
+    <t>unusual.jpeg</t>
+  </si>
+  <si>
+    <t>mooi.jpeg</t>
+  </si>
+  <si>
+    <t>negen.jpeg</t>
+  </si>
+  <si>
+    <t>vikingShake.jpeg</t>
+  </si>
+  <si>
+    <t>treeblood.jpeg</t>
+  </si>
+  <si>
+    <t>cocoaShake.jpeg</t>
+  </si>
+  <si>
+    <t>george.jpeg</t>
+  </si>
+  <si>
+    <t>clock.jpeg</t>
+  </si>
+  <si>
+    <t>slope.jpeg</t>
+  </si>
+  <si>
+    <t>sourbon.jpeg</t>
+  </si>
+  <si>
+    <t>funken.jpeg</t>
+  </si>
+  <si>
+    <t>geuzeboon.jpeg</t>
+  </si>
+  <si>
+    <t>anno1521.jpeg</t>
+  </si>
+  <si>
+    <t>GCImperial.jpeg</t>
+  </si>
+  <si>
+    <t>GCClassic.jpeg</t>
+  </si>
+  <si>
+    <t>GCAmbrio.jpeg</t>
+  </si>
+  <si>
+    <t>browneyes.jpeg</t>
+  </si>
+  <si>
+    <t>pleasure.jpeg</t>
+  </si>
+  <si>
+    <t>sexyblond.jpeg</t>
+  </si>
+  <si>
+    <t>poppelsStout.jpeg</t>
+  </si>
+  <si>
+    <t>poppelsBA.jpeg</t>
+  </si>
+  <si>
+    <t>poppelsRhum.jpeg</t>
+  </si>
+  <si>
+    <t>heavyhitter.jpeg</t>
+  </si>
+  <si>
+    <t>hwg.jpeg</t>
+  </si>
+  <si>
+    <t>oudegueuze.jpeg</t>
+  </si>
+  <si>
+    <t>quetsche.jpeg</t>
+  </si>
+  <si>
+    <t>baristaen.jpeg</t>
+  </si>
+  <si>
+    <t>elskerinden.jpeg</t>
+  </si>
+  <si>
+    <t>psykopaten.jpeg</t>
+  </si>
+  <si>
+    <t>agenten.jpeg</t>
+  </si>
+  <si>
+    <t>fyrbøderen.jpeg</t>
+  </si>
+  <si>
+    <t>vandervelden.jpeg</t>
+  </si>
+  <si>
+    <t>duchesse.jpeg</t>
+  </si>
+  <si>
+    <t>GCInfused.jpeg</t>
+  </si>
+  <si>
+    <t>mirror.jpeg</t>
+  </si>
+  <si>
+    <t>ponder.jpeg</t>
+  </si>
+  <si>
+    <t>dwell.jpeg</t>
+  </si>
+  <si>
+    <t>paradox.jpeg</t>
+  </si>
+  <si>
+    <t>romanoid.jpeg</t>
+  </si>
+  <si>
+    <t>doubledippy.jpeg</t>
+  </si>
+  <si>
+    <t>space.jpeg</t>
+  </si>
+  <si>
+    <t>illusion.jpeg</t>
+  </si>
+  <si>
+    <t>tonka.jpeg</t>
+  </si>
+  <si>
+    <t>berrypavlova.jpeg</t>
+  </si>
+  <si>
+    <t>bbpie.jpeg</t>
+  </si>
+  <si>
+    <t>toffee.jpeg</t>
+  </si>
+  <si>
+    <t>cheesecake.jpeg</t>
+  </si>
+  <si>
+    <t>bairischpils.jpeg</t>
+  </si>
+  <si>
+    <t>keller.jpeg</t>
+  </si>
+  <si>
+    <t>urweisse.jpeg</t>
+  </si>
+  <si>
+    <t>celebrator.jpeg</t>
+  </si>
+  <si>
+    <t>weissbier.jpeg</t>
+  </si>
+  <si>
+    <t>aventinusdb.jpeg</t>
+  </si>
+  <si>
+    <t>aventinuseb.jpeg</t>
+  </si>
+  <si>
+    <t>dvana.jpeg</t>
+  </si>
+  <si>
+    <t>tmava.jpeg</t>
+  </si>
+  <si>
+    <t>ris.jpeg</t>
+  </si>
+  <si>
+    <t>chilitripel.jpeg</t>
+  </si>
+  <si>
+    <t>winterw2021.jpeg</t>
+  </si>
+  <si>
+    <t>soulwarmer.jpeg</t>
+  </si>
+  <si>
+    <t>brownbourbon.jpeg</t>
+  </si>
+  <si>
+    <t>farmhouse.jpeg</t>
+  </si>
+  <si>
+    <t>saisonbuck.jpeg</t>
+  </si>
+  <si>
+    <t>BAStrong.jpeg</t>
+  </si>
+  <si>
+    <t>blacknight.jpeg</t>
   </si>
 </sst>
 </file>
@@ -534,7 +1155,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -830,22 +1451,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E550A8CF-F9F0-4525-B5C7-3366B4AD2A8A}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="128" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" zoomScale="128" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -871,7 +1493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -893,8 +1515,11 @@
       <c r="G2">
         <v>330</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -913,8 +1538,11 @@
       <c r="G3">
         <v>700</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -933,8 +1561,11 @@
       <c r="G4">
         <v>440</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -953,8 +1584,11 @@
       <c r="G5">
         <v>375</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -973,8 +1607,11 @@
       <c r="G6">
         <v>375</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -993,8 +1630,11 @@
       <c r="G7">
         <v>330</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -1002,7 +1642,7 @@
         <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D8" t="s">
         <v>40</v>
@@ -1013,8 +1653,11 @@
       <c r="G8">
         <v>375</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -1022,7 +1665,7 @@
         <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D9" t="s">
         <v>40</v>
@@ -1033,8 +1676,11 @@
       <c r="G9">
         <v>375</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -1042,7 +1688,7 @@
         <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D10" t="s">
         <v>40</v>
@@ -1053,8 +1699,11 @@
       <c r="G10">
         <v>375</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>71</v>
       </c>
@@ -1073,8 +1722,11 @@
       <c r="G11">
         <v>500</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>76</v>
       </c>
@@ -1093,8 +1745,11 @@
       <c r="G12">
         <v>500</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -1113,8 +1768,11 @@
       <c r="G13">
         <v>500</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -1130,8 +1788,11 @@
       <c r="G14">
         <v>500</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>88</v>
       </c>
@@ -1150,8 +1811,11 @@
       <c r="G15">
         <v>500</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>89</v>
       </c>
@@ -1167,8 +1831,11 @@
       <c r="G16">
         <v>750</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>91</v>
       </c>
@@ -1187,8 +1854,11 @@
       <c r="G17">
         <v>500</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>92</v>
       </c>
@@ -1207,8 +1877,11 @@
       <c r="G18">
         <v>500</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>93</v>
       </c>
@@ -1227,8 +1900,11 @@
       <c r="G19">
         <v>500</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1741</v>
       </c>
@@ -1247,13 +1923,16 @@
       <c r="G20">
         <v>500</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D21" t="s">
         <v>87</v>
@@ -1267,10 +1946,13 @@
       <c r="G21">
         <v>500</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
         <v>47</v>
@@ -1287,16 +1969,19 @@
       <c r="G22">
         <v>500</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" t="s">
         <v>100</v>
-      </c>
-      <c r="C23" t="s">
-        <v>101</v>
-      </c>
-      <c r="D23" t="s">
-        <v>99</v>
       </c>
       <c r="E23">
         <v>5.5</v>
@@ -1307,16 +1992,19 @@
       <c r="G23">
         <v>500</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C24" t="s">
         <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E24">
         <v>15</v>
@@ -1327,16 +2015,19 @@
       <c r="G24">
         <v>500</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D25" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E25">
         <v>5</v>
@@ -1347,16 +2038,19 @@
       <c r="G25">
         <v>500</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D26" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E26">
         <v>7.4</v>
@@ -1364,16 +2058,19 @@
       <c r="G26">
         <v>500</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D27" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E27">
         <v>9.3000000000000007</v>
@@ -1384,16 +2081,19 @@
       <c r="G27">
         <v>500</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>110</v>
+        <v>161</v>
       </c>
       <c r="C28" t="s">
         <v>53</v>
       </c>
       <c r="D28" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E28">
         <v>10.1</v>
@@ -1404,8 +2104,11 @@
       <c r="G28">
         <v>500</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -1413,7 +2116,7 @@
         <v>53</v>
       </c>
       <c r="D29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E29">
         <v>12</v>
@@ -1424,16 +2127,19 @@
       <c r="G29">
         <v>500</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>600</v>
       </c>
       <c r="C30" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D30" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E30">
         <v>12.7</v>
@@ -1444,8 +2150,11 @@
       <c r="G30">
         <v>330</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -1461,10 +2170,13 @@
       <c r="G31">
         <v>330</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C32" t="s">
         <v>114</v>
@@ -1478,10 +2190,13 @@
       <c r="G32">
         <v>330</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H32" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C33" t="s">
         <v>114</v>
@@ -1495,10 +2210,13 @@
       <c r="G33">
         <v>330</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C34" t="s">
         <v>114</v>
@@ -1512,10 +2230,13 @@
       <c r="G34">
         <v>330</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H34" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C35" t="s">
         <v>114</v>
@@ -1529,8 +2250,11 @@
       <c r="G35">
         <v>330</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H35" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>120</v>
       </c>
@@ -1546,8 +2270,11 @@
       <c r="G36">
         <v>440</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H36" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>122</v>
       </c>
@@ -1563,8 +2290,11 @@
       <c r="G37">
         <v>440</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>123</v>
       </c>
@@ -1580,8 +2310,11 @@
       <c r="G38">
         <v>440</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>126</v>
       </c>
@@ -1597,8 +2330,11 @@
       <c r="G39">
         <v>440</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>128</v>
       </c>
@@ -1614,13 +2350,16 @@
       <c r="G40">
         <v>440</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>130</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D41" t="s">
         <v>129</v>
@@ -1631,8 +2370,11 @@
       <c r="G41">
         <v>330</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>131</v>
       </c>
@@ -1648,8 +2390,11 @@
       <c r="G42">
         <v>330</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>133</v>
       </c>
@@ -1665,8 +2410,11 @@
       <c r="G43">
         <v>330</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H43" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>135</v>
       </c>
@@ -1682,8 +2430,11 @@
       <c r="G44">
         <v>330</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H44" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>136</v>
       </c>
@@ -1699,13 +2450,16 @@
       <c r="G45">
         <v>330</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H45" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>138</v>
       </c>
       <c r="C46" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D46" t="s">
         <v>139</v>
@@ -1716,8 +2470,11 @@
       <c r="G46">
         <v>473</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H46" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>140</v>
       </c>
@@ -1733,8 +2490,11 @@
       <c r="G47">
         <v>473</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H47" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>142</v>
       </c>
@@ -1750,8 +2510,11 @@
       <c r="G48">
         <v>330</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>141</v>
       </c>
@@ -1767,13 +2530,16 @@
       <c r="G49">
         <v>473</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H49" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>145</v>
       </c>
       <c r="C50" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D50" t="s">
         <v>144</v>
@@ -1783,6 +2549,1173 @@
       </c>
       <c r="G50">
         <v>330</v>
+      </c>
+      <c r="H50" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>163</v>
+      </c>
+      <c r="C51" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" t="s">
+        <v>162</v>
+      </c>
+      <c r="E51">
+        <v>10</v>
+      </c>
+      <c r="G51">
+        <v>375</v>
+      </c>
+      <c r="H51" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>164</v>
+      </c>
+      <c r="C52" t="s">
+        <v>166</v>
+      </c>
+      <c r="D52" t="s">
+        <v>162</v>
+      </c>
+      <c r="E52">
+        <v>7</v>
+      </c>
+      <c r="G52">
+        <v>375</v>
+      </c>
+      <c r="H52" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>169</v>
+      </c>
+      <c r="C53" t="s">
+        <v>171</v>
+      </c>
+      <c r="D53" t="s">
+        <v>90</v>
+      </c>
+      <c r="E53">
+        <v>8</v>
+      </c>
+      <c r="G53">
+        <v>750</v>
+      </c>
+      <c r="H53" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>165</v>
+      </c>
+      <c r="C54" t="s">
+        <v>167</v>
+      </c>
+      <c r="D54" t="s">
+        <v>168</v>
+      </c>
+      <c r="E54">
+        <v>7</v>
+      </c>
+      <c r="G54">
+        <v>750</v>
+      </c>
+      <c r="H54" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>170</v>
+      </c>
+      <c r="C55" t="s">
+        <v>172</v>
+      </c>
+      <c r="D55" t="s">
+        <v>90</v>
+      </c>
+      <c r="E55">
+        <v>8.5</v>
+      </c>
+      <c r="G55">
+        <v>750</v>
+      </c>
+      <c r="H55" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>173</v>
+      </c>
+      <c r="C56" t="s">
+        <v>174</v>
+      </c>
+      <c r="D56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E56">
+        <v>11</v>
+      </c>
+      <c r="G56">
+        <v>750</v>
+      </c>
+      <c r="H56" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>175</v>
+      </c>
+      <c r="C57" t="s">
+        <v>102</v>
+      </c>
+      <c r="D57" t="s">
+        <v>90</v>
+      </c>
+      <c r="E57">
+        <v>8.5</v>
+      </c>
+      <c r="G57">
+        <v>330</v>
+      </c>
+      <c r="H57" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>176</v>
+      </c>
+      <c r="C58" t="s">
+        <v>171</v>
+      </c>
+      <c r="D58" t="s">
+        <v>90</v>
+      </c>
+      <c r="E58">
+        <v>8</v>
+      </c>
+      <c r="G58">
+        <v>330</v>
+      </c>
+      <c r="H58" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>178</v>
+      </c>
+      <c r="C59" t="s">
+        <v>102</v>
+      </c>
+      <c r="D59" t="s">
+        <v>177</v>
+      </c>
+      <c r="E59">
+        <v>12</v>
+      </c>
+      <c r="G59">
+        <v>330</v>
+      </c>
+      <c r="H59" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>182</v>
+      </c>
+      <c r="C60" t="s">
+        <v>183</v>
+      </c>
+      <c r="D60" t="s">
+        <v>177</v>
+      </c>
+      <c r="E60">
+        <v>8</v>
+      </c>
+      <c r="G60">
+        <v>330</v>
+      </c>
+      <c r="H60" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>184</v>
+      </c>
+      <c r="C61" t="s">
+        <v>172</v>
+      </c>
+      <c r="D61" t="s">
+        <v>177</v>
+      </c>
+      <c r="E61">
+        <v>8</v>
+      </c>
+      <c r="G61">
+        <v>330</v>
+      </c>
+      <c r="H61" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>180</v>
+      </c>
+      <c r="C62" t="s">
+        <v>103</v>
+      </c>
+      <c r="D62" t="s">
+        <v>179</v>
+      </c>
+      <c r="E62">
+        <v>13.2</v>
+      </c>
+      <c r="F62">
+        <v>30</v>
+      </c>
+      <c r="G62">
+        <v>330</v>
+      </c>
+      <c r="H62" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" t="s">
+        <v>181</v>
+      </c>
+      <c r="D63" t="s">
+        <v>179</v>
+      </c>
+      <c r="E63">
+        <v>13.5</v>
+      </c>
+      <c r="F63">
+        <v>25</v>
+      </c>
+      <c r="G63">
+        <v>330</v>
+      </c>
+      <c r="H63" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>186</v>
+      </c>
+      <c r="C64" t="s">
+        <v>181</v>
+      </c>
+      <c r="D64" t="s">
+        <v>179</v>
+      </c>
+      <c r="E64">
+        <v>12.5</v>
+      </c>
+      <c r="F64">
+        <v>25</v>
+      </c>
+      <c r="G64">
+        <v>330</v>
+      </c>
+      <c r="H64" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>187</v>
+      </c>
+      <c r="C65" t="s">
+        <v>125</v>
+      </c>
+      <c r="D65" t="s">
+        <v>188</v>
+      </c>
+      <c r="E65">
+        <v>10.5</v>
+      </c>
+      <c r="G65">
+        <v>440</v>
+      </c>
+      <c r="H65" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>189</v>
+      </c>
+      <c r="C66" t="s">
+        <v>190</v>
+      </c>
+      <c r="D66" t="s">
+        <v>191</v>
+      </c>
+      <c r="E66">
+        <v>6.4</v>
+      </c>
+      <c r="G66">
+        <v>440</v>
+      </c>
+      <c r="H66" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>193</v>
+      </c>
+      <c r="C67" t="s">
+        <v>166</v>
+      </c>
+      <c r="D67" t="s">
+        <v>192</v>
+      </c>
+      <c r="E67">
+        <v>7</v>
+      </c>
+      <c r="G67">
+        <v>375</v>
+      </c>
+      <c r="H67" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>194</v>
+      </c>
+      <c r="C68" t="s">
+        <v>166</v>
+      </c>
+      <c r="D68" t="s">
+        <v>192</v>
+      </c>
+      <c r="E68">
+        <v>6.4</v>
+      </c>
+      <c r="G68">
+        <v>375</v>
+      </c>
+      <c r="H68" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>195</v>
+      </c>
+      <c r="C69" t="s">
+        <v>44</v>
+      </c>
+      <c r="D69" t="s">
+        <v>31</v>
+      </c>
+      <c r="E69">
+        <v>8</v>
+      </c>
+      <c r="F69">
+        <v>40</v>
+      </c>
+      <c r="G69">
+        <v>330</v>
+      </c>
+      <c r="H69" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>196</v>
+      </c>
+      <c r="C70" t="s">
+        <v>44</v>
+      </c>
+      <c r="D70" t="s">
+        <v>31</v>
+      </c>
+      <c r="E70">
+        <v>10</v>
+      </c>
+      <c r="F70">
+        <v>50</v>
+      </c>
+      <c r="G70">
+        <v>330</v>
+      </c>
+      <c r="H70" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>197</v>
+      </c>
+      <c r="C71" t="s">
+        <v>190</v>
+      </c>
+      <c r="D71" t="s">
+        <v>31</v>
+      </c>
+      <c r="E71">
+        <v>5.8</v>
+      </c>
+      <c r="F71">
+        <v>500</v>
+      </c>
+      <c r="G71">
+        <v>330</v>
+      </c>
+      <c r="H71" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>198</v>
+      </c>
+      <c r="C72" t="s">
+        <v>190</v>
+      </c>
+      <c r="D72" t="s">
+        <v>31</v>
+      </c>
+      <c r="E72">
+        <v>7.5</v>
+      </c>
+      <c r="F72">
+        <v>70</v>
+      </c>
+      <c r="G72">
+        <v>330</v>
+      </c>
+      <c r="H72" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>199</v>
+      </c>
+      <c r="C73" t="s">
+        <v>53</v>
+      </c>
+      <c r="D73" t="s">
+        <v>31</v>
+      </c>
+      <c r="E73">
+        <v>11.5</v>
+      </c>
+      <c r="F73">
+        <v>70</v>
+      </c>
+      <c r="G73">
+        <v>330</v>
+      </c>
+      <c r="H73" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>201</v>
+      </c>
+      <c r="C74" t="s">
+        <v>114</v>
+      </c>
+      <c r="D74" t="s">
+        <v>200</v>
+      </c>
+      <c r="E74">
+        <v>6.5</v>
+      </c>
+      <c r="G74">
+        <v>375</v>
+      </c>
+      <c r="H74" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>203</v>
+      </c>
+      <c r="C75" t="s">
+        <v>50</v>
+      </c>
+      <c r="D75" t="s">
+        <v>202</v>
+      </c>
+      <c r="E75">
+        <v>6.2</v>
+      </c>
+      <c r="G75">
+        <v>250</v>
+      </c>
+      <c r="H75" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>204</v>
+      </c>
+      <c r="C76" t="s">
+        <v>102</v>
+      </c>
+      <c r="D76" t="s">
+        <v>90</v>
+      </c>
+      <c r="E76">
+        <v>11.7</v>
+      </c>
+      <c r="G76">
+        <v>330</v>
+      </c>
+      <c r="H76" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>206</v>
+      </c>
+      <c r="C77" t="s">
+        <v>96</v>
+      </c>
+      <c r="D77" t="s">
+        <v>205</v>
+      </c>
+      <c r="E77">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="G77">
+        <v>440</v>
+      </c>
+      <c r="H77" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>207</v>
+      </c>
+      <c r="C78" t="s">
+        <v>127</v>
+      </c>
+      <c r="D78" t="s">
+        <v>205</v>
+      </c>
+      <c r="E78">
+        <v>7.5</v>
+      </c>
+      <c r="G78">
+        <v>440</v>
+      </c>
+      <c r="H78" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>208</v>
+      </c>
+      <c r="C79" t="s">
+        <v>127</v>
+      </c>
+      <c r="D79" t="s">
+        <v>205</v>
+      </c>
+      <c r="E79">
+        <v>6</v>
+      </c>
+      <c r="G79">
+        <v>440</v>
+      </c>
+      <c r="H79" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>209</v>
+      </c>
+      <c r="C80" t="s">
+        <v>210</v>
+      </c>
+      <c r="D80" t="s">
+        <v>205</v>
+      </c>
+      <c r="E80">
+        <v>5.5</v>
+      </c>
+      <c r="G80">
+        <v>440</v>
+      </c>
+      <c r="H80" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>211</v>
+      </c>
+      <c r="C81" t="s">
+        <v>127</v>
+      </c>
+      <c r="D81" t="s">
+        <v>205</v>
+      </c>
+      <c r="E81">
+        <v>7.5</v>
+      </c>
+      <c r="G81">
+        <v>440</v>
+      </c>
+      <c r="H81" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>212</v>
+      </c>
+      <c r="C82" t="s">
+        <v>127</v>
+      </c>
+      <c r="D82" t="s">
+        <v>205</v>
+      </c>
+      <c r="E82">
+        <v>7.5</v>
+      </c>
+      <c r="G82">
+        <v>440</v>
+      </c>
+      <c r="H82" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>247</v>
+      </c>
+      <c r="C83" t="s">
+        <v>125</v>
+      </c>
+      <c r="D83" t="s">
+        <v>205</v>
+      </c>
+      <c r="E83">
+        <v>10</v>
+      </c>
+      <c r="G83">
+        <v>440</v>
+      </c>
+      <c r="H83" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>213</v>
+      </c>
+      <c r="C84" t="s">
+        <v>127</v>
+      </c>
+      <c r="D84" t="s">
+        <v>205</v>
+      </c>
+      <c r="E84">
+        <v>7.5</v>
+      </c>
+      <c r="G84">
+        <v>440</v>
+      </c>
+      <c r="H84" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>216</v>
+      </c>
+      <c r="C85" t="s">
+        <v>181</v>
+      </c>
+      <c r="D85" t="s">
+        <v>214</v>
+      </c>
+      <c r="E85">
+        <v>11.5</v>
+      </c>
+      <c r="G85">
+        <v>330</v>
+      </c>
+      <c r="H85" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>215</v>
+      </c>
+      <c r="C86" t="s">
+        <v>44</v>
+      </c>
+      <c r="D86" t="s">
+        <v>214</v>
+      </c>
+      <c r="E86">
+        <v>10.5</v>
+      </c>
+      <c r="G86">
+        <v>330</v>
+      </c>
+      <c r="H86" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>217</v>
+      </c>
+      <c r="C87" t="s">
+        <v>181</v>
+      </c>
+      <c r="D87" t="s">
+        <v>214</v>
+      </c>
+      <c r="E87">
+        <v>11.5</v>
+      </c>
+      <c r="G87">
+        <v>330</v>
+      </c>
+      <c r="H87" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>218</v>
+      </c>
+      <c r="C88" t="s">
+        <v>181</v>
+      </c>
+      <c r="D88" t="s">
+        <v>214</v>
+      </c>
+      <c r="E88">
+        <v>11.5</v>
+      </c>
+      <c r="G88">
+        <v>330</v>
+      </c>
+      <c r="H88" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>219</v>
+      </c>
+      <c r="C89" t="s">
+        <v>44</v>
+      </c>
+      <c r="D89" t="s">
+        <v>214</v>
+      </c>
+      <c r="E89">
+        <v>10.5</v>
+      </c>
+      <c r="G89">
+        <v>330</v>
+      </c>
+      <c r="H89" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>220</v>
+      </c>
+      <c r="C90" t="s">
+        <v>223</v>
+      </c>
+      <c r="D90" t="s">
+        <v>86</v>
+      </c>
+      <c r="E90">
+        <v>5.3</v>
+      </c>
+      <c r="G90">
+        <v>330</v>
+      </c>
+      <c r="H90" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>221</v>
+      </c>
+      <c r="C91" t="s">
+        <v>221</v>
+      </c>
+      <c r="D91" t="s">
+        <v>86</v>
+      </c>
+      <c r="E91">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G91">
+        <v>500</v>
+      </c>
+      <c r="H91" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>222</v>
+      </c>
+      <c r="C92" t="s">
+        <v>222</v>
+      </c>
+      <c r="D92" t="s">
+        <v>86</v>
+      </c>
+      <c r="E92">
+        <v>5.8</v>
+      </c>
+      <c r="G92">
+        <v>500</v>
+      </c>
+      <c r="H92" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>224</v>
+      </c>
+      <c r="C93" t="s">
+        <v>225</v>
+      </c>
+      <c r="D93" t="s">
+        <v>86</v>
+      </c>
+      <c r="E93">
+        <v>6.7</v>
+      </c>
+      <c r="G93">
+        <v>330</v>
+      </c>
+      <c r="H93" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>227</v>
+      </c>
+      <c r="C94" t="s">
+        <v>228</v>
+      </c>
+      <c r="D94" t="s">
+        <v>226</v>
+      </c>
+      <c r="E94">
+        <v>5.4</v>
+      </c>
+      <c r="G94">
+        <v>500</v>
+      </c>
+      <c r="H94" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>229</v>
+      </c>
+      <c r="C95" t="s">
+        <v>225</v>
+      </c>
+      <c r="D95" t="s">
+        <v>226</v>
+      </c>
+      <c r="E95">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G95">
+        <v>500</v>
+      </c>
+      <c r="H95" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>230</v>
+      </c>
+      <c r="C96" t="s">
+        <v>225</v>
+      </c>
+      <c r="D96" t="s">
+        <v>226</v>
+      </c>
+      <c r="E96">
+        <v>12</v>
+      </c>
+      <c r="G96">
+        <v>330</v>
+      </c>
+      <c r="H96" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>232</v>
+      </c>
+      <c r="C97" t="s">
+        <v>85</v>
+      </c>
+      <c r="D97" t="s">
+        <v>231</v>
+      </c>
+      <c r="E97">
+        <v>5.2</v>
+      </c>
+      <c r="G97">
+        <v>500</v>
+      </c>
+      <c r="H97" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>233</v>
+      </c>
+      <c r="C98" t="s">
+        <v>44</v>
+      </c>
+      <c r="D98" t="s">
+        <v>231</v>
+      </c>
+      <c r="E98">
+        <v>5.9</v>
+      </c>
+      <c r="G98">
+        <v>500</v>
+      </c>
+      <c r="H98" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>235</v>
+      </c>
+      <c r="C99" t="s">
+        <v>121</v>
+      </c>
+      <c r="D99" t="s">
+        <v>234</v>
+      </c>
+      <c r="E99">
+        <v>11</v>
+      </c>
+      <c r="G99">
+        <v>500</v>
+      </c>
+      <c r="H99" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>236</v>
+      </c>
+      <c r="C100" t="s">
+        <v>125</v>
+      </c>
+      <c r="D100" t="s">
+        <v>234</v>
+      </c>
+      <c r="E100">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G100">
+        <v>500</v>
+      </c>
+      <c r="H100" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>238</v>
+      </c>
+      <c r="C101" t="s">
+        <v>114</v>
+      </c>
+      <c r="D101" t="s">
+        <v>237</v>
+      </c>
+      <c r="E101">
+        <v>8</v>
+      </c>
+      <c r="G101">
+        <v>375</v>
+      </c>
+      <c r="H101" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>239</v>
+      </c>
+      <c r="C102" t="s">
+        <v>114</v>
+      </c>
+      <c r="D102" t="s">
+        <v>237</v>
+      </c>
+      <c r="E102">
+        <v>10.3</v>
+      </c>
+      <c r="G102">
+        <v>375</v>
+      </c>
+      <c r="H102" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>240</v>
+      </c>
+      <c r="C103" t="s">
+        <v>114</v>
+      </c>
+      <c r="D103" t="s">
+        <v>237</v>
+      </c>
+      <c r="E103">
+        <v>5.3</v>
+      </c>
+      <c r="G103">
+        <v>750</v>
+      </c>
+      <c r="H103" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>241</v>
+      </c>
+      <c r="C104" t="s">
+        <v>190</v>
+      </c>
+      <c r="D104" t="s">
+        <v>237</v>
+      </c>
+      <c r="E104">
+        <v>7.5</v>
+      </c>
+      <c r="G104">
+        <v>750</v>
+      </c>
+      <c r="H104" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>242</v>
+      </c>
+      <c r="C105" t="s">
+        <v>243</v>
+      </c>
+      <c r="D105" t="s">
+        <v>237</v>
+      </c>
+      <c r="E105">
+        <v>5.2</v>
+      </c>
+      <c r="G105">
+        <v>750</v>
+      </c>
+      <c r="H105" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>244</v>
+      </c>
+      <c r="C106" t="s">
+        <v>114</v>
+      </c>
+      <c r="D106" t="s">
+        <v>237</v>
+      </c>
+      <c r="E106">
+        <v>10</v>
+      </c>
+      <c r="G106">
+        <v>375</v>
+      </c>
+      <c r="H106" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>245</v>
+      </c>
+      <c r="C107" t="s">
+        <v>246</v>
+      </c>
+      <c r="D107" t="s">
+        <v>237</v>
+      </c>
+      <c r="E107">
+        <v>5.2</v>
+      </c>
+      <c r="G107">
+        <v>375</v>
+      </c>
+      <c r="H107" t="s">
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -1792,19 +3725,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D18B146-37B4-4384-8640-C656446A1852}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView zoomScale="194" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A12" zoomScale="194" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1812,7 +3745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1820,7 +3753,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1828,7 +3761,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1836,7 +3769,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -1844,7 +3777,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1852,7 +3785,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -1860,49 +3793,124 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -1914,20 +3922,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4BA013A-79D9-4770-B0BB-271DCEC96FBB}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView zoomScale="167" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1950,7 +3958,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1969,8 +3977,11 @@
       <c r="F2">
         <v>700</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1989,8 +4000,11 @@
       <c r="F3">
         <v>500</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2009,8 +4023,11 @@
       <c r="F4">
         <v>700</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2029,8 +4046,11 @@
       <c r="F5">
         <v>700</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2049,8 +4069,11 @@
       <c r="F6">
         <v>700</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2069,8 +4092,11 @@
       <c r="F7">
         <v>700</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -2089,8 +4115,11 @@
       <c r="F8">
         <v>700</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -2109,8 +4138,11 @@
       <c r="F9">
         <v>700</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -2129,8 +4161,11 @@
       <c r="F10">
         <v>700</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2149,8 +4184,11 @@
       <c r="F11">
         <v>700</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -2169,8 +4207,11 @@
       <c r="F12">
         <v>700</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -2189,8 +4230,11 @@
       <c r="F13">
         <v>700</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -2209,8 +4253,11 @@
       <c r="F14">
         <v>700</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -2228,6 +4275,9 @@
       </c>
       <c r="F15">
         <v>700</v>
+      </c>
+      <c r="G15" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2243,13 +4293,13 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2257,7 +4307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2265,7 +4315,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -2273,7 +4323,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>

</xml_diff>